<commit_message>
- [DOC_02] Ajout d'une colonne d'identifiant unique pour la gestion des doublons
</commit_message>
<xml_diff>
--- a/Source/GSoft.Dynamite.CrossSitePublishingCMS/Modules/Docs/DOC_02/Default/ContentPages.xlsx
+++ b/Source/GSoft.Dynamite.CrossSitePublishingCMS/Modules/Docs/DOC_02/Default/ContentPages.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -31,15 +31,6 @@
   </si>
   <si>
     <t>Title</t>
-  </si>
-  <si>
-    <t>Navigation</t>
-  </si>
-  <si>
-    <t>Page Content</t>
-  </si>
-  <si>
-    <t>Publishing Start Date</t>
   </si>
   <si>
     <t>1_.000</t>
@@ -112,6 +103,18 @@
   </si>
   <si>
     <t>Modified</t>
+  </si>
+  <si>
+    <t>DynamiteNavigation</t>
+  </si>
+  <si>
+    <t>PublishingPageContent</t>
+  </si>
+  <si>
+    <t>DynamitePublishingStartDate</t>
+  </si>
+  <si>
+    <t>DynamiteInternalId</t>
   </si>
 </sst>
 </file>
@@ -155,11 +158,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,28 +468,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15"/>
-    <col min="2" max="6" width="15" style="3"/>
+    <col min="2" max="5" width="15" style="3"/>
+    <col min="6" max="6" width="22" style="3" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="15" style="3"/>
-    <col min="9" max="9" width="15" style="1"/>
-    <col min="10" max="11" width="15" style="3"/>
-    <col min="12" max="12" width="15" style="1"/>
-    <col min="13" max="13" width="15" style="3"/>
-    <col min="14" max="14" width="15" style="1"/>
-    <col min="15" max="21" width="15" style="3"/>
+    <col min="8" max="8" width="27.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="3"/>
+    <col min="10" max="10" width="15" style="1"/>
+    <col min="11" max="12" width="15" style="3"/>
+    <col min="13" max="13" width="15" style="1"/>
+    <col min="14" max="14" width="15" style="3"/>
+    <col min="15" max="15" width="15" style="1"/>
+    <col min="16" max="22" width="15" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -499,30 +505,32 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -531,33 +539,36 @@
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="G2" s="1">
         <v>41936</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2"/>
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
@@ -569,9 +580,11 @@
       <c r="S2"/>
       <c r="T2"/>
       <c r="U2"/>
-      <c r="W2" s="3"/>
+      <c r="V2"/>
+      <c r="X2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- [DOC_02] Ajout de valeurs pour la colonne "OccurenceLinkLocation" dans les fichiers Excel d'import
</commit_message>
<xml_diff>
--- a/Source/GSoft.Dynamite.CrossSitePublishingCMS/Modules/Docs/DOC_02/Default/ContentPages.xlsx
+++ b/Source/GSoft.Dynamite.CrossSitePublishingCMS/Modules/Docs/DOC_02/Default/ContentPages.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>DynamiteInternalId</t>
+  </si>
+  <si>
+    <t>DynamiteOccurrenceLinkLocation</t>
+  </si>
+  <si>
+    <t>Main Menu</t>
   </si>
 </sst>
 </file>
@@ -158,12 +164,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,30 +475,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15"/>
-    <col min="2" max="5" width="15" style="3"/>
-    <col min="6" max="6" width="22" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="3"/>
-    <col min="10" max="10" width="15" style="1"/>
-    <col min="11" max="12" width="15" style="3"/>
-    <col min="13" max="13" width="15" style="1"/>
-    <col min="14" max="14" width="15" style="3"/>
-    <col min="15" max="15" width="15" style="1"/>
-    <col min="16" max="22" width="15" style="3"/>
+    <col min="2" max="4" width="15" style="3"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="34.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="3"/>
+    <col min="11" max="11" width="15" style="1"/>
+    <col min="12" max="13" width="15" style="3"/>
+    <col min="14" max="14" width="15" style="1"/>
+    <col min="15" max="15" width="15" style="3"/>
+    <col min="16" max="16" width="15" style="1"/>
+    <col min="17" max="23" width="15" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -513,25 +522,27 @@
       <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -540,8 +551,9 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -563,13 +575,15 @@
       <c r="G2" s="1">
         <v>41936</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="4">
         <v>1</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
       <c r="N2"/>
@@ -581,7 +595,8 @@
       <c r="T2"/>
       <c r="U2"/>
       <c r="V2"/>
-      <c r="X2" s="3"/>
+      <c r="W2"/>
+      <c r="Y2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- [DOC_02] Ajout de contenu supplémentaire + images + termes de navigation pour effectuer les tests fonctionnels de base.
</commit_message>
<xml_diff>
--- a/Source/GSoft.Dynamite.CrossSitePublishingCMS/Modules/Docs/DOC_02/Default/ContentPages.xlsx
+++ b/Source/GSoft.Dynamite.CrossSitePublishingCMS/Modules/Docs/DOC_02/Default/ContentPages.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -39,51 +39,6 @@
     <t>About Us</t>
   </si>
   <si>
-    <t>About</t>
-  </si>
-  <si>
-    <t>&lt;h1&gt;​One morning, when Gregor Samsa woke from troubled 
-dreams.&lt;/h1&gt;&lt;p&gt;One morning, when Gregor Samsa woke from troubled 
-dreams, he found himself transformed in his bed into 
-a horrible vermin. He lay on his armour-like back, 
-and if he lifted his head a little he could see his 
-brown belly, slightly domed and divided by arches into 
-stiff sections. The bedding was hardly able to cover 
-&lt;strong&gt;strong&lt;/strong&gt; it and seemed ready to slide 
-off any moment. His many legs, pitifully thin 
-compared with the size of the rest of him, 
-&lt;a class="external ext" href="#"&gt;link&lt;/a&gt; waved about 
-helplessly as he looked. &amp;quot;What's happened to me? &amp;quot; he 
-thought. It wasn't a dream. His room, a proper human 
-room although a little too small, lay peacefully 
-between its four familiar walls.&lt;/p&gt;&lt;h1&gt;One morning, when Gregor Samsa woke from troubled 
-dreams.&lt;/h1&gt;&lt;h2&gt;The bedding was hardly able to cover it.&lt;/h2&gt;&lt;p&gt;It showed a lady fitted out with a fur hat and fur 
-boa who sat upright, raising a heavy fur muff that 
-covered the whole of her lower arm towards the 
-viewer.&lt;/p&gt;&lt;h2&gt;The bedding was hardly able to cover it.&lt;/h2&gt;&lt;p&gt;It showed a lady fitted out with a fur hat and fur 
-boa who sat upright, raising a heavy fur muff that 
-covered the whole of her lower arm towards the 
-viewer.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Lorem ipsum dolor sit amet consectetuer.&lt;/li&gt;&lt;li&gt;Aenean commodo ligula eget dolor.&lt;/li&gt;&lt;li&gt;Aenean massa cum sociis natoque penatibus.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;It showed a lady fitted out with a fur hat and fur 
-boa who sat upright, raising a heavy fur muff that 
-covered the whole of her lower arm towards the 
-viewer.&lt;/p&gt;&lt;fieldset&gt;
-    &lt;label&gt;Name&amp;#58;&lt;/label&gt;
-    &lt;input type="text" id="name" placeholder="Enter your   full name" /&gt;
-    &lt;label&gt;Email&amp;#58;&lt;/label&gt;
-    &lt;input type="email" id="email" placeholder="Enter   your email address" /&gt;
-    &lt;label&gt;Message&amp;#58;&lt;/label&gt;
-    &lt;textarea id="message" placeholder="What's on your   mind?"&gt;&lt;/textarea&gt;
-    &lt;input type="button" value="Send message" /&gt;
-  &lt;/fieldset&gt;&lt;p&gt;It showed a lady fitted out with a fur hat and fur 
-boa who sat upright, raising a heavy fur muff that 
-covered the whole of her lower arm towards the 
-viewer.&lt;/p&gt;&lt;table class="data"&gt;&lt;tbody&gt;&lt;tr&gt;&lt;th&gt;Entry Header 1&lt;/th&gt;&lt;th&gt;Entry Header 2&lt;/th&gt;&lt;th&gt;Entry Header 3&lt;/th&gt;&lt;th&gt;Entry Header 4&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Entry First Line 1&lt;/td&gt;&lt;td&gt;Entry First Line 2&lt;/td&gt;&lt;td&gt;Entry First Line 3&lt;/td&gt;&lt;td&gt;Entry First Line 4&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Entry Line 1&lt;/td&gt;&lt;td&gt;Entry Line 2&lt;/td&gt;&lt;td&gt;Entry Line 3&lt;/td&gt;&lt;td&gt;Entry Line 4&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Entry Last Line 1&lt;/td&gt;&lt;td&gt;Entry Last Line 2&lt;/td&gt;&lt;td&gt;Entry Last Line 3&lt;/td&gt;&lt;td&gt;Entry Last Line 4&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;p&gt;It showed a lady fitted out with a fur hat and fur 
-boa who sat upright, raising a heavy fur muff that 
-covered the whole of her lower arm towards the 
-viewer.&lt;/p&gt;
-​</t>
-  </si>
-  <si>
     <t>Content Item</t>
   </si>
   <si>
@@ -121,6 +76,97 @@
   </si>
   <si>
     <t>Main Menu</t>
+  </si>
+  <si>
+    <t>About us</t>
+  </si>
+  <si>
+    <t>2_.000</t>
+  </si>
+  <si>
+    <t>Our history</t>
+  </si>
+  <si>
+    <t>3_.000</t>
+  </si>
+  <si>
+    <t>Our culture</t>
+  </si>
+  <si>
+    <t>4_.000</t>
+  </si>
+  <si>
+    <t>Our philosophy</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>5_.000</t>
+  </si>
+  <si>
+    <t>6_.000</t>
+  </si>
+  <si>
+    <t>Contact us</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Fifth replenish upon. Years divide. I us called thing dry waters he itself. Female very she&amp;#39;d, whales stars the darkness i Beast fruit that of. Two &lt;strong&gt;behold&lt;/strong&gt; moving.&lt;/p&gt;
+&lt;p&gt;Moved yielding upon you every us beginning place sea &lt;em&gt;creature&lt;/em&gt; him good.&lt;/p&gt;
+&lt;p&gt;There hath, first lights air that &lt;em&gt;him&lt;/em&gt; dominion midst very. Abundantly is dominion face place forth. Sea said grass it divided stars divide.&lt;/p&gt;
+&lt;p&gt;One. Creeping shall. Fly that &lt;em&gt;they&amp;#39;re&lt;/em&gt; stars divide air second moveth winged.&lt;/p&gt;
+&lt;p&gt;Darkness meat all. Fruit evening our &lt;strong&gt;don&amp;#39;t&lt;/strong&gt; third you he blessed. Gathered.&lt;/p&gt;
+&lt;p&gt;Living image fruit from all can&amp;#39;t can&amp;#39;t beginning given place earth shall lights.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Brought deep. Likeness kind won&amp;#39;t fly kind doesn&amp;#39;t seas sixth in greater won&amp;#39;t land, seasons, midst it. Winged. Let.&lt;/p&gt;
+&lt;p&gt;Firmament &lt;em&gt;of&lt;/em&gt; gathering greater fowl had that isn&amp;#39;t forth which every second seas was &lt;em&gt;fourth&lt;/em&gt; seed itself, let a them. Their.&lt;/p&gt;
+&lt;p&gt;Replenish given them man make god forth life.&lt;/p&gt;
+&lt;p&gt;There female &lt;strong&gt;tree&lt;/strong&gt; that may saw. Forth dry that subdue dry second, seed place moved own called give fruit you seed shall called don&amp;#39;t them moving.&lt;/p&gt;
+&lt;p&gt;Wherein saw brought, beast thing saw saw fowl one bring beast that.&lt;/p&gt;
+&lt;p&gt;Make which be air, replenish greater form morning years void don&amp;#39;t. To &lt;strong&gt;from&lt;/strong&gt; lesser.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Isn&amp;#39;t bearing fifth gathered was third land unto us brought image also had subdue thing fruit.&lt;/p&gt;
+&lt;p&gt;Seas first. Made from creature, image seasons void sea &lt;em&gt;they&amp;#39;re&lt;/em&gt; second.&lt;/p&gt;
+&lt;p&gt;May bearing two don&amp;#39;t make fowl under. Abundantly whales days grass thing brought in.&lt;/p&gt;
+&lt;p&gt;Fill bring creeping there. Created made set second multiply first one you&amp;#39;re so seas multiply tree void.&lt;/p&gt;
+&lt;p&gt;Divided the unto stars isn&amp;#39;t, replenish divided God. Man from above. Spirit spirit bearing dry. Life behold good.&lt;/p&gt;
+&lt;p&gt;Creature given, heaven, given divide, have kind appear together, can&amp;#39;t. Tree void don&amp;#39;t and there they&amp;#39;re have Whales. &lt;em&gt;Two&lt;/em&gt; &lt;em&gt;lights&lt;/em&gt; all heaven his all.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Meat life replenish. One.&lt;/p&gt;
+&lt;p&gt;Seasons forth The blessed Fifth. After.&lt;/p&gt;
+&lt;p&gt;Night heaven &lt;em&gt;third&lt;/em&gt; morning appear.&lt;/p&gt;
+&lt;p&gt;Midst female deep two.&lt;/p&gt;
+&lt;p&gt;I, deep face, years beast. Can&amp;#39;t air.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Subdue&lt;/strong&gt; given replenish lesser.&lt;/p&gt;
+&lt;p&gt;They&amp;#39;re seas there. One. Unto the fruit.&lt;/p&gt;
+&lt;p&gt;Firmament. Moving you&amp;#39;ll open, &lt;strong&gt;lights&lt;/strong&gt; beginning. Won&amp;#39;t, signs.&lt;/p&gt;
+&lt;p&gt;Winged doesn&amp;#39;t behold you&amp;#39;ll.&lt;/p&gt;
+&lt;p&gt;Morning wherein light. Winged which fowl it.&lt;/p&gt;
+&lt;p&gt;In meat kind kind creeping all.&lt;/p&gt;
+&lt;p&gt;Seas signs moveth divided brought.&lt;/p&gt;
+&lt;p&gt;Fish living i gathered, fruit wherein unto fill.&lt;/p&gt;
+&lt;p&gt;Place &lt;strong&gt;rule&lt;/strong&gt; night beast lesser signs male.&lt;/p&gt;
+&lt;p&gt;Whose years forth place, whose was.&lt;/p&gt;
+&lt;p&gt;Male. Very called. Over &lt;strong&gt;in&lt;/strong&gt; god fourth have fruit good hath whales.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Is &lt;em&gt;have&lt;/em&gt; waters. First it created &lt;strong&gt;their&lt;/strong&gt; sea sea years, behold god. Called.&lt;/p&gt;
+&lt;p&gt;All air. Years fifth over. Days was beast had sixth behold evening don&amp;#39;t. Stars every set. Itself yielding man together of called.&lt;/p&gt;
+&lt;p&gt;Darkness land make set morning above won&amp;#39;t that.&lt;/p&gt;
+&lt;p&gt;Beginning together form male fruit moveth bring first green fourth all creeping. Greater every likeness have fruitful &lt;em&gt;blessed&lt;/em&gt; every also.&lt;/p&gt;
+&lt;p&gt;Shall. Lesser given saying, light creature had likeness &lt;em&gt;so&lt;/em&gt; herb void beginning. For very land Female given. Thing, place don&amp;#39;t one.&lt;/p&gt;
+&lt;p&gt;They&amp;#39;re life creature. Light upon made evening won&amp;#39;t night so meat, waters firmament let fill. The.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Unto have place his. After days let replenish, life created so The. For given.&lt;/p&gt;
+&lt;p&gt;Firmament to for moving Beast. Kind fruitful set from there and he had sixth. Can&amp;#39;t great. Two every saw &lt;em&gt;fill&lt;/em&gt; first gathered.&lt;/p&gt;
+&lt;p&gt;Green creepeth beginning sixth third forth without. Be moved, make together shall, beast hath good creeping blessed saying cattle. They&amp;#39;re created won&amp;#39;t.&lt;/p&gt;
+&lt;p&gt;Lights man thing fill fruitful. Isn&amp;#39;t evening wherein firmament them over void given a greater to greater sixth darkness.&lt;/p&gt;
+&lt;p&gt;Forth. Form also fowl two and day created.&lt;/p&gt;
+&lt;p&gt;Is you&amp;#39;re fill void deep may moved moving said moved The evening were replenish. Place.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -164,13 +210,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,19 +524,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15"/>
     <col min="2" max="4" width="15" style="3"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
-    <col min="6" max="6" width="34.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="100.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="31.140625" style="3" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" style="3" customWidth="1"/>
     <col min="9" max="9" width="27.85546875" style="1" customWidth="1"/>
@@ -514,34 +563,34 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -553,7 +602,7 @@
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -561,28 +610,28 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="G2" s="1">
         <v>41936</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I2" s="4">
         <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L2"/>
       <c r="M2"/>
@@ -598,6 +647,231 @@
       <c r="W2"/>
       <c r="Y2" s="3"/>
     </row>
+    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="1">
+        <v>41936</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="4">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="Y3" s="3"/>
+    </row>
+    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1">
+        <v>41936</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="4">
+        <v>3</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="Y4" s="3"/>
+    </row>
+    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="1">
+        <v>41936</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="4">
+        <v>4</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="Y5" s="3"/>
+    </row>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1">
+        <v>41936</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="4">
+        <v>5</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="Y6" s="3"/>
+    </row>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="1">
+        <v>41936</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="4">
+        <v>6</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="Y7" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>